<commit_message>
Finished The CRUD Categories
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -1202,7 +1202,7 @@
     </x:row>
     <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="2" t="s">
-        <x:v>41</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
         <x:v>75</x:v>
@@ -1219,7 +1219,7 @@
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="2" t="s">
-        <x:v>43</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
         <x:v>75</x:v>
@@ -1236,7 +1236,7 @@
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="2" t="s">
-        <x:v>45</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
         <x:v>75</x:v>
@@ -1253,7 +1253,7 @@
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="2" t="s">
-        <x:v>47</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
         <x:v>75</x:v>
@@ -1270,7 +1270,7 @@
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="2" t="s">
-        <x:v>49</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
         <x:v>75</x:v>

</xml_diff>

<commit_message>
Finished Version one with the addition of Device CRUD testing
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming_And_Stuff\Programming\Git\CMPG-323-Project-4-34551875\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F7388D-0C33-410B-9038-E4F2CF3FFF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE6E0BD-BA95-4E4B-BDC3-5A8E56912AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-19320" yWindow="1875" windowWidth="19440" windowHeight="15150" firstSheet="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="28680" yWindow="4560" windowWidth="20730" windowHeight="11310" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -707,8 +707,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:F10"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="C38" sqref="C38"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F14" sqref="F14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:E24"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="F8" sqref="F8"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1202,7 +1202,7 @@
     </x:row>
     <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A2" s="2" t="s">
-        <x:v>61</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
         <x:v>75</x:v>
@@ -1219,7 +1219,7 @@
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="2" t="s">
-        <x:v>63</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
         <x:v>75</x:v>
@@ -1236,7 +1236,7 @@
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="2" t="s">
-        <x:v>65</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
         <x:v>75</x:v>
@@ -1253,7 +1253,7 @@
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="2" t="s">
-        <x:v>67</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
         <x:v>75</x:v>
@@ -1270,7 +1270,7 @@
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="2" t="s">
-        <x:v>69</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B6" s="2" t="s">
         <x:v>75</x:v>
@@ -1354,102 +1354,242 @@
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="2" t="s"/>
-      <x:c r="B11" s="2" t="s"/>
-      <x:c r="C11" s="2" t="s"/>
-      <x:c r="D11" s="2" t="s"/>
-      <x:c r="E11" s="2" t="s"/>
+      <x:c r="A11" s="2" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B11" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C11" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D11" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E11" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="2" t="s"/>
-      <x:c r="B12" s="2" t="s"/>
-      <x:c r="C12" s="2" t="s"/>
-      <x:c r="D12" s="2" t="s"/>
-      <x:c r="E12" s="2" t="s"/>
+      <x:c r="A12" s="2" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E12" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="2" t="s"/>
-      <x:c r="B13" s="2" t="s"/>
-      <x:c r="C13" s="2" t="s"/>
-      <x:c r="D13" s="2" t="s"/>
-      <x:c r="E13" s="2" t="s"/>
+      <x:c r="A13" s="2" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E13" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="2" t="s"/>
-      <x:c r="B14" s="2" t="s"/>
-      <x:c r="C14" s="2" t="s"/>
-      <x:c r="D14" s="2" t="s"/>
-      <x:c r="E14" s="2" t="s"/>
+      <x:c r="A14" s="2" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E14" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="2" t="s"/>
-      <x:c r="B15" s="2" t="s"/>
-      <x:c r="C15" s="2" t="s"/>
-      <x:c r="D15" s="2" t="s"/>
-      <x:c r="E15" s="2" t="s"/>
+      <x:c r="A15" s="2" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E15" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="2" t="s"/>
-      <x:c r="B16" s="2" t="s"/>
-      <x:c r="C16" s="2" t="s"/>
-      <x:c r="D16" s="2" t="s"/>
-      <x:c r="E16" s="2" t="s"/>
+      <x:c r="A16" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E16" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A17" s="2" t="s"/>
-      <x:c r="B17" s="2" t="s"/>
-      <x:c r="C17" s="2" t="s"/>
-      <x:c r="D17" s="2" t="s"/>
-      <x:c r="E17" s="2" t="s"/>
+      <x:c r="A17" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E17" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A18" s="2" t="s"/>
-      <x:c r="B18" s="2" t="s"/>
-      <x:c r="C18" s="2" t="s"/>
-      <x:c r="D18" s="2" t="s"/>
-      <x:c r="E18" s="2" t="s"/>
+      <x:c r="A18" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E18" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A19" s="2" t="s"/>
-      <x:c r="B19" s="2" t="s"/>
-      <x:c r="C19" s="2" t="s"/>
-      <x:c r="D19" s="2" t="s"/>
-      <x:c r="E19" s="2" t="s"/>
+      <x:c r="A19" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E19" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A20" s="2" t="s"/>
-      <x:c r="B20" s="2" t="s"/>
-      <x:c r="C20" s="2" t="s"/>
-      <x:c r="D20" s="2" t="s"/>
-      <x:c r="E20" s="2" t="s"/>
+      <x:c r="A20" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E20" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A21" s="2" t="s"/>
-      <x:c r="B21" s="2" t="s"/>
-      <x:c r="C21" s="2" t="s"/>
-      <x:c r="D21" s="2" t="s"/>
-      <x:c r="E21" s="2" t="s"/>
+      <x:c r="A21" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E21" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A22" s="2" t="s"/>
-      <x:c r="B22" s="2" t="s"/>
-      <x:c r="C22" s="2" t="s"/>
-      <x:c r="D22" s="2" t="s"/>
-      <x:c r="E22" s="2" t="s"/>
+      <x:c r="A22" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E22" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A23" s="2" t="s"/>
-      <x:c r="B23" s="2" t="s"/>
-      <x:c r="C23" s="2" t="s"/>
-      <x:c r="D23" s="2" t="s"/>
-      <x:c r="E23" s="2" t="s"/>
+      <x:c r="A23" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E23" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
     <x:row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A24" s="2" t="s"/>
-      <x:c r="B24" s="2" t="s"/>
-      <x:c r="C24" s="2" t="s"/>
-      <x:c r="D24" s="2" t="s"/>
-      <x:c r="E24" s="2" t="s"/>
+      <x:c r="A24" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="C24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="D24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E24" s="2" t="s">
+        <x:v>75</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>